<commit_message>
Interim temporal test data
</commit_message>
<xml_diff>
--- a/data/testdata/all_cases.xlsx
+++ b/data/testdata/all_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/juan_russy_urosario_edu_co/Documents/initial_graph_repository/namegraph/data/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="800" documentId="8_{80136A59-A22F-4BFD-841B-785D5A5637AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32D490BE-C711-452B-BCCE-A623E2E078F1}"/>
+  <xr:revisionPtr revIDLastSave="823" documentId="8_{80136A59-A22F-4BFD-841B-785D5A5637AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7C87239-DEE9-415E-B2A0-C4345834E5FF}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="6435" windowWidth="21600" windowHeight="8760" xr2:uid="{181804AA-FA84-4F41-B5A6-3D72BBD7180C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{181804AA-FA84-4F41-B5A6-3D72BBD7180C}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL_CASES" sheetId="1" r:id="rId1"/>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A0D0B-AFBE-4BC1-B10F-8C3D3610350B}">
   <dimension ref="A1:W97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8050,7 +8050,7 @@
   <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>